<commit_message>
Update DaneTelefonow — kopia.xlsx
</commit_message>
<xml_diff>
--- a/DaneTelefonow — kopia.xlsx
+++ b/DaneTelefonow — kopia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RMapps\Git\Statystyczna-analiza-danych\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFDBB7ED-EC3D-4015-A851-233BD6AA39F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD368F05-93B6-49B7-8FC9-4AB1E38A8FB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="40">
   <si>
     <t>Telefon\zmienne</t>
   </si>
@@ -169,6 +169,12 @@
   </si>
   <si>
     <t>d0</t>
+  </si>
+  <si>
+    <t>wagi:</t>
+  </si>
+  <si>
+    <t>model:</t>
   </si>
 </sst>
 </file>
@@ -1030,10 +1036,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AS27"/>
+  <dimension ref="A1:AS50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
-      <selection activeCell="AU18" sqref="AU18"/>
+    <sheetView tabSelected="1" topLeftCell="AE26" zoomScale="90" workbookViewId="0">
+      <selection activeCell="AS28" sqref="AS28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1048,6 +1054,7 @@
     <col min="8" max="8" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="27.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:45" x14ac:dyDescent="0.3">
@@ -1307,7 +1314,7 @@
         <v>9.2833887072095713</v>
       </c>
       <c r="AS2" cm="1">
-        <f t="array" ref="AS2:AS24">1-AP2:AP24/$AQ$2</f>
+        <f t="array" ref="AS2:AS24">1-(AP2:AP24/$AQ$2)</f>
         <v>0.27420644734871003</v>
       </c>
     </row>
@@ -1433,7 +1440,7 @@
         <v>14.350597052355416</v>
       </c>
       <c r="AP3">
-        <f t="shared" ref="AP3:AP24" si="10">SQRT(SUM(AF3:AN3))</f>
+        <f t="shared" ref="AP3:AP50" si="10">SQRT(SUM(AF3:AN3))</f>
         <v>6.5974509616026804</v>
       </c>
       <c r="AS3">
@@ -4228,6 +4235,37 @@
         <f t="shared" si="12"/>
         <v>3.6279051879960242</v>
       </c>
+      <c r="AE26" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF26">
+        <v>0.17</v>
+      </c>
+      <c r="AG26">
+        <v>0.21</v>
+      </c>
+      <c r="AH26">
+        <v>0.1</v>
+      </c>
+      <c r="AI26">
+        <v>0.09</v>
+      </c>
+      <c r="AJ26">
+        <v>0.04</v>
+      </c>
+      <c r="AK26">
+        <v>0.08</v>
+      </c>
+      <c r="AL26">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="AM26">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="AN26">
+        <f>1-SUM(AF26:AM26)</f>
+        <v>0.16000000000000014</v>
+      </c>
     </row>
     <row r="27" spans="1:45" x14ac:dyDescent="0.3">
       <c r="K27" t="s">
@@ -4268,6 +4306,918 @@
       <c r="T27">
         <f t="shared" si="13"/>
         <v>39.596452076079146</v>
+      </c>
+      <c r="AE27" t="s">
+        <v>39</v>
+      </c>
+      <c r="AP27" t="s">
+        <v>36</v>
+      </c>
+      <c r="AQ27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AE28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AF28" cm="1">
+        <f t="array" ref="AF28:AN50">AF$26:AN$26*AF2:AN24</f>
+        <v>0.36720778221764033</v>
+      </c>
+      <c r="AG28">
+        <v>0.42842906030960715</v>
+      </c>
+      <c r="AH28">
+        <v>1.0189653548027497</v>
+      </c>
+      <c r="AI28">
+        <v>0.41258155819680903</v>
+      </c>
+      <c r="AJ28">
+        <v>0.22282173955144927</v>
+      </c>
+      <c r="AK28">
+        <v>0.43077314503176384</v>
+      </c>
+      <c r="AL28">
+        <v>4.688601325013856E-2</v>
+      </c>
+      <c r="AM28">
+        <v>1.005433567371762E-3</v>
+      </c>
+      <c r="AN28">
+        <v>2.3577329372275186</v>
+      </c>
+      <c r="AP28">
+        <f t="shared" si="10"/>
+        <v>2.2992179157607153</v>
+      </c>
+      <c r="AQ28">
+        <f t="shared" ref="AQ3:AQ28" si="14">AVERAGE(AP28:AP50)+2*_xlfn.STDEV.P(AP28:AP50)</f>
+        <v>3.1389434406530969</v>
+      </c>
+      <c r="AS28" cm="1">
+        <f t="array" ref="AS28:AS50">1-(AP28:AP50/$AQ$28)</f>
+        <v>0.26751852678099419</v>
+      </c>
+    </row>
+    <row r="29" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AE29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF29">
+        <v>0.11601814504172195</v>
+      </c>
+      <c r="AG29">
+        <v>5.0221872848004126E-2</v>
+      </c>
+      <c r="AH29">
+        <v>1.0189653548027497</v>
+      </c>
+      <c r="AI29">
+        <v>0.26405219724595774</v>
+      </c>
+      <c r="AJ29">
+        <v>0.39960232329845008</v>
+      </c>
+      <c r="AK29">
+        <v>6.1295580940860975E-2</v>
+      </c>
+      <c r="AL29">
+        <v>0.27741176576049842</v>
+      </c>
+      <c r="AM29">
+        <v>9.0489021063458689E-3</v>
+      </c>
+      <c r="AN29">
+        <v>2.2960955283768687</v>
+      </c>
+      <c r="AP29">
+        <f t="shared" si="10"/>
+        <v>2.1196017716593505</v>
+      </c>
+      <c r="AS29">
+        <v>0.3247403746725871</v>
+      </c>
+    </row>
+    <row r="30" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AE30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF30">
+        <v>0.57827107880178985</v>
+      </c>
+      <c r="AG30">
+        <v>1.1642656394118923E-2</v>
+      </c>
+      <c r="AH30">
+        <v>1.0189653548027497</v>
+      </c>
+      <c r="AI30">
+        <v>0.26405219724595774</v>
+      </c>
+      <c r="AJ30">
+        <v>0.19910980814870866</v>
+      </c>
+      <c r="AK30">
+        <v>6.1295580940860975E-2</v>
+      </c>
+      <c r="AL30">
+        <v>0.34248366143271414</v>
+      </c>
+      <c r="AM30">
+        <v>1.6086937077948213E-2</v>
+      </c>
+      <c r="AN30">
+        <v>0.86374011343030266</v>
+      </c>
+      <c r="AP30">
+        <f t="shared" si="10"/>
+        <v>1.8318426210444911</v>
+      </c>
+      <c r="AS30">
+        <v>0.41641426305427376</v>
+      </c>
+    </row>
+    <row r="31" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AE31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF31">
+        <v>1.0280374734254036</v>
+      </c>
+      <c r="AG31">
+        <v>2.4922201385793021E-2</v>
+      </c>
+      <c r="AH31">
+        <v>0.74177521704309268</v>
+      </c>
+      <c r="AI31">
+        <v>0.26405219724595774</v>
+      </c>
+      <c r="AJ31">
+        <v>0.15163793468346953</v>
+      </c>
+      <c r="AK31">
+        <v>0.55166022846774876</v>
+      </c>
+      <c r="AL31">
+        <v>0.34248366143271414</v>
+      </c>
+      <c r="AM31">
+        <v>0</v>
+      </c>
+      <c r="AN31">
+        <v>2.2960955283768687</v>
+      </c>
+      <c r="AP31">
+        <f t="shared" si="10"/>
+        <v>2.3239329684956593</v>
+      </c>
+      <c r="AS31">
+        <v>0.25964484151006695</v>
+      </c>
+    </row>
+    <row r="32" spans="1:45" x14ac:dyDescent="0.3">
+      <c r="AE32" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF32">
+        <v>2.2770835522446444</v>
+      </c>
+      <c r="AG32">
+        <v>5.5480134625260887E-3</v>
+      </c>
+      <c r="AH32">
+        <v>1.0189653548027497</v>
+      </c>
+      <c r="AI32">
+        <v>0.26405219724595774</v>
+      </c>
+      <c r="AJ32">
+        <v>0.290714146967125</v>
+      </c>
+      <c r="AK32">
+        <v>0.15691668720860411</v>
+      </c>
+      <c r="AL32">
+        <v>0.57879738782128687</v>
+      </c>
+      <c r="AM32">
+        <v>4.0217342694870515E-3</v>
+      </c>
+      <c r="AN32">
+        <v>2.2960955283768687</v>
+      </c>
+      <c r="AP32">
+        <f t="shared" si="10"/>
+        <v>2.6252989548619503</v>
+      </c>
+      <c r="AS32">
+        <v>0.16363610734071599</v>
+      </c>
+    </row>
+    <row r="33" spans="31:45" x14ac:dyDescent="0.3">
+      <c r="AE33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF33">
+        <v>0.26510365754530846</v>
+      </c>
+      <c r="AG33">
+        <v>0.11033658661469485</v>
+      </c>
+      <c r="AH33">
+        <v>1.0189653548027497</v>
+      </c>
+      <c r="AI33">
+        <v>6.6013049311489436E-2</v>
+      </c>
+      <c r="AJ33">
+        <v>0.45354496679552808</v>
+      </c>
+      <c r="AK33">
+        <v>6.0928359115444274E-2</v>
+      </c>
+      <c r="AL33">
+        <v>0.16781699410202994</v>
+      </c>
+      <c r="AM33">
+        <v>6.4347748311792852E-2</v>
+      </c>
+      <c r="AN33">
+        <v>2.2960955283768687</v>
+      </c>
+      <c r="AP33">
+        <f t="shared" si="10"/>
+        <v>2.1220632047551993</v>
+      </c>
+      <c r="AS33">
+        <v>0.32395621492508409</v>
+      </c>
+    </row>
+    <row r="34" spans="31:45" x14ac:dyDescent="0.3">
+      <c r="AE34" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF34">
+        <v>0.16641921318924119</v>
+      </c>
+      <c r="AG34">
+        <v>7.502279771121606E-2</v>
+      </c>
+      <c r="AH34">
+        <v>0.74177521704309268</v>
+      </c>
+      <c r="AI34">
+        <v>6.6013049311489436E-2</v>
+      </c>
+      <c r="AJ34">
+        <v>0.41943072577853707</v>
+      </c>
+      <c r="AK34">
+        <v>0.1201393386440875</v>
+      </c>
+      <c r="AL34">
+        <v>0.27741176576049842</v>
+      </c>
+      <c r="AM34">
+        <v>4.0217342694870515E-3</v>
+      </c>
+      <c r="AN34">
+        <v>0.86374011343030266</v>
+      </c>
+      <c r="AP34">
+        <f t="shared" si="10"/>
+        <v>1.6534733004006905</v>
+      </c>
+      <c r="AS34">
+        <v>0.47323889975645295</v>
+      </c>
+    </row>
+    <row r="35" spans="31:45" x14ac:dyDescent="0.3">
+      <c r="AE35" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF35">
+        <v>1.4023983484146807</v>
+      </c>
+      <c r="AG35">
+        <v>1.5459270721318608E-2</v>
+      </c>
+      <c r="AH35">
+        <v>1.0189653548027497</v>
+      </c>
+      <c r="AI35">
+        <v>0.26405219724595774</v>
+      </c>
+      <c r="AJ35">
+        <v>0.42278213655553848</v>
+      </c>
+      <c r="AK35">
+        <v>0.13426184049286188</v>
+      </c>
+      <c r="AL35">
+        <v>0.34248366143271414</v>
+      </c>
+      <c r="AM35">
+        <v>3.6195608425383476E-2</v>
+      </c>
+      <c r="AN35">
+        <v>1.8874925730159362</v>
+      </c>
+      <c r="AP35">
+        <f t="shared" si="10"/>
+        <v>2.3503384843692494</v>
+      </c>
+      <c r="AS35">
+        <v>0.25123261097045069</v>
+      </c>
+    </row>
+    <row r="36" spans="31:45" x14ac:dyDescent="0.3">
+      <c r="AE36" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AF36">
+        <v>1.411794625981054E-4</v>
+      </c>
+      <c r="AG36">
+        <v>2.5802882227685701E-3</v>
+      </c>
+      <c r="AH36">
+        <v>1.2556747546222593</v>
+      </c>
+      <c r="AI36">
+        <v>0.59411744380340481</v>
+      </c>
+      <c r="AJ36">
+        <v>0.17673150618369257</v>
+      </c>
+      <c r="AK36">
+        <v>0.55166022846774876</v>
+      </c>
+      <c r="AL36">
+        <v>0.34248366143271414</v>
+      </c>
+      <c r="AM36">
+        <v>0.90489021063458674</v>
+      </c>
+      <c r="AN36">
+        <v>3.6068089046645353</v>
+      </c>
+      <c r="AP36">
+        <f t="shared" si="10"/>
+        <v>2.7267358099922894</v>
+      </c>
+      <c r="AS36">
+        <v>0.13132050272783591</v>
+      </c>
+    </row>
+    <row r="37" spans="31:45" x14ac:dyDescent="0.3">
+      <c r="AE37" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AF37">
+        <v>0.62746427821374773</v>
+      </c>
+      <c r="AG37">
+        <v>0.32818239929651194</v>
+      </c>
+      <c r="AH37">
+        <v>0.31912886837985288</v>
+      </c>
+      <c r="AI37">
+        <v>0</v>
+      </c>
+      <c r="AJ37">
+        <v>0.3076619098617272</v>
+      </c>
+      <c r="AK37">
+        <v>4.9649420562097382E-2</v>
+      </c>
+      <c r="AL37">
+        <v>0.16781699410202994</v>
+      </c>
+      <c r="AM37">
+        <v>1.005433567371762E-3</v>
+      </c>
+      <c r="AN37">
+        <v>0</v>
+      </c>
+      <c r="AP37">
+        <f t="shared" si="10"/>
+        <v>1.3419796212995707</v>
+      </c>
+      <c r="AS37">
+        <v>0.57247409943125482</v>
+      </c>
+    </row>
+    <row r="38" spans="31:45" x14ac:dyDescent="0.3">
+      <c r="AE38" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AF38">
+        <v>5.4605078811551334E-2</v>
+      </c>
+      <c r="AG38">
+        <v>0.21588932283252477</v>
+      </c>
+      <c r="AH38">
+        <v>1.0189653548027497</v>
+      </c>
+      <c r="AI38">
+        <v>0.26405219724595774</v>
+      </c>
+      <c r="AJ38">
+        <v>0.20374550407423883</v>
+      </c>
+      <c r="AK38">
+        <v>0.27031351194919695</v>
+      </c>
+      <c r="AL38">
+        <v>6.0414117876730761E-2</v>
+      </c>
+      <c r="AM38">
+        <v>9.0489021063458689E-3</v>
+      </c>
+      <c r="AN38">
+        <v>2.2960955283768687</v>
+      </c>
+      <c r="AP38">
+        <f t="shared" si="10"/>
+        <v>2.0959793696685485</v>
+      </c>
+      <c r="AS38">
+        <v>0.33226596487114357</v>
+      </c>
+    </row>
+    <row r="39" spans="31:45" x14ac:dyDescent="0.3">
+      <c r="AE39" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AF39">
+        <v>0.64007631020584388</v>
+      </c>
+      <c r="AG39">
+        <v>3.1851001379893442</v>
+      </c>
+      <c r="AH39">
+        <v>0</v>
+      </c>
+      <c r="AI39">
+        <v>0</v>
+      </c>
+      <c r="AJ39">
+        <v>0.73853624311949007</v>
+      </c>
+      <c r="AK39">
+        <v>6.1295580940860975E-2</v>
+      </c>
+      <c r="AL39">
+        <v>0.21374405310015684</v>
+      </c>
+      <c r="AM39">
+        <v>1.005433567371762E-3</v>
+      </c>
+      <c r="AN39">
+        <v>2.3577329372275186</v>
+      </c>
+      <c r="AP39">
+        <f t="shared" si="10"/>
+        <v>2.682813951087661</v>
+      </c>
+      <c r="AS39">
+        <v>0.14531306415337397</v>
+      </c>
+    </row>
+    <row r="40" spans="31:45" x14ac:dyDescent="0.3">
+      <c r="AE40" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF40">
+        <v>5.4605078811551334E-2</v>
+      </c>
+      <c r="AG40">
+        <v>2.360359821312819</v>
+      </c>
+      <c r="AH40">
+        <v>0</v>
+      </c>
+      <c r="AI40">
+        <v>0.26405219724595774</v>
+      </c>
+      <c r="AJ40">
+        <v>0.53329067265369878</v>
+      </c>
+      <c r="AK40">
+        <v>0.15263114537154288</v>
+      </c>
+      <c r="AL40">
+        <v>1.58313072497272E-2</v>
+      </c>
+      <c r="AM40">
+        <v>1.005433567371762E-3</v>
+      </c>
+      <c r="AN40">
+        <v>2.3577329372275186</v>
+      </c>
+      <c r="AP40">
+        <f t="shared" si="10"/>
+        <v>2.3957271533795721</v>
+      </c>
+      <c r="AS40">
+        <v>0.23677275533161224</v>
+      </c>
+    </row>
+    <row r="41" spans="31:45" x14ac:dyDescent="0.3">
+      <c r="AE41" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF41">
+        <v>1.7394721586711051</v>
+      </c>
+      <c r="AG41">
+        <v>0.18200847625447594</v>
+      </c>
+      <c r="AH41">
+        <v>1.0189653548027497</v>
+      </c>
+      <c r="AI41">
+        <v>0.59411744380340481</v>
+      </c>
+      <c r="AJ41">
+        <v>0.23768904052320128</v>
+      </c>
+      <c r="AK41">
+        <v>0.2247846868158489</v>
+      </c>
+      <c r="AL41">
+        <v>8.2230327109994658E-2</v>
+      </c>
+      <c r="AM41">
+        <v>8.1440118957112825E-2</v>
+      </c>
+      <c r="AN41">
+        <v>3.6068089046645353</v>
+      </c>
+      <c r="AP41">
+        <f t="shared" si="10"/>
+        <v>2.7870264641015572</v>
+      </c>
+      <c r="AS41">
+        <v>0.11211319452073942</v>
+      </c>
+    </row>
+    <row r="42" spans="31:45" x14ac:dyDescent="0.3">
+      <c r="AE42" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF42">
+        <v>0.61497773907729392</v>
+      </c>
+      <c r="AG42">
+        <v>1.0764290305213504</v>
+      </c>
+      <c r="AH42">
+        <v>0.31912886837985288</v>
+      </c>
+      <c r="AI42">
+        <v>0</v>
+      </c>
+      <c r="AJ42">
+        <v>0.73853624311949007</v>
+      </c>
+      <c r="AK42">
+        <v>0</v>
+      </c>
+      <c r="AL42">
+        <v>0</v>
+      </c>
+      <c r="AM42">
+        <v>4.0217342694870515E-3</v>
+      </c>
+      <c r="AN42">
+        <v>2.2960955283768687</v>
+      </c>
+      <c r="AP42">
+        <f t="shared" si="10"/>
+        <v>2.2470400850328289</v>
+      </c>
+      <c r="AS42">
+        <v>0.28414126360769854</v>
+      </c>
+    </row>
+    <row r="43" spans="31:45" x14ac:dyDescent="0.3">
+      <c r="AE43" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF43">
+        <v>5.2769745797776171E-2</v>
+      </c>
+      <c r="AG43">
+        <v>0.38751445098768611</v>
+      </c>
+      <c r="AH43">
+        <v>0.31912886837985288</v>
+      </c>
+      <c r="AI43">
+        <v>0</v>
+      </c>
+      <c r="AJ43">
+        <v>0.67770673720600305</v>
+      </c>
+      <c r="AK43">
+        <v>0</v>
+      </c>
+      <c r="AL43">
+        <v>8.5620915358178534E-2</v>
+      </c>
+      <c r="AM43">
+        <v>4.0217342694870515E-3</v>
+      </c>
+      <c r="AN43">
+        <v>2.2960955283768687</v>
+      </c>
+      <c r="AP43">
+        <f t="shared" si="10"/>
+        <v>1.9552130268530465</v>
+      </c>
+      <c r="AS43">
+        <v>0.37711110001834258</v>
+      </c>
+    </row>
+    <row r="44" spans="31:45" x14ac:dyDescent="0.3">
+      <c r="AE44" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF44">
+        <v>0.28166871449015141</v>
+      </c>
+      <c r="AG44">
+        <v>3.6443581257330847E-2</v>
+      </c>
+      <c r="AH44">
+        <v>1.0189653548027497</v>
+      </c>
+      <c r="AI44">
+        <v>0.41258155819680903</v>
+      </c>
+      <c r="AJ44">
+        <v>0.36138583813101849</v>
+      </c>
+      <c r="AK44">
+        <v>0.13426184049286188</v>
+      </c>
+      <c r="AL44">
+        <v>8.5620915358178534E-2</v>
+      </c>
+      <c r="AM44">
+        <v>0.12165746165198338</v>
+      </c>
+      <c r="AN44">
+        <v>2.3577329372275186</v>
+      </c>
+      <c r="AP44">
+        <f t="shared" si="10"/>
+        <v>2.1932437624688692</v>
+      </c>
+      <c r="AS44">
+        <v>0.30127961719101981</v>
+      </c>
+    </row>
+    <row r="45" spans="31:45" x14ac:dyDescent="0.3">
+      <c r="AE45" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF45">
+        <v>0.36720778221764033</v>
+      </c>
+      <c r="AG45">
+        <v>1.3119689252639097E-2</v>
+      </c>
+      <c r="AH45">
+        <v>1.0189653548027497</v>
+      </c>
+      <c r="AI45">
+        <v>0.26405219724595774</v>
+      </c>
+      <c r="AJ45">
+        <v>0.22772416136452425</v>
+      </c>
+      <c r="AK45">
+        <v>0.23909107540744587</v>
+      </c>
+      <c r="AL45">
+        <v>0.37758823672956726</v>
+      </c>
+      <c r="AM45">
+        <v>0.1447824337015339</v>
+      </c>
+      <c r="AN45">
+        <v>2.3577329372275186</v>
+      </c>
+      <c r="AP45">
+        <f t="shared" si="10"/>
+        <v>2.2383618715367666</v>
+      </c>
+      <c r="AS45">
+        <v>0.28690595614203007</v>
+      </c>
+    </row>
+    <row r="46" spans="31:45" x14ac:dyDescent="0.3">
+      <c r="AE46" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF46">
+        <v>4.5334294100943268E-3</v>
+      </c>
+      <c r="AG46">
+        <v>0.12385030745024402</v>
+      </c>
+      <c r="AH46">
+        <v>0.74177521704309268</v>
+      </c>
+      <c r="AI46">
+        <v>6.6013049311489436E-2</v>
+      </c>
+      <c r="AJ46">
+        <v>0.41276791310766575</v>
+      </c>
+      <c r="AK46">
+        <v>4.3250161911871504E-2</v>
+      </c>
+      <c r="AL46">
+        <v>8.5620915358178534E-2</v>
+      </c>
+      <c r="AM46">
+        <v>4.0217342694870515E-3</v>
+      </c>
+      <c r="AN46">
+        <v>1.8874925730159362</v>
+      </c>
+      <c r="AP46">
+        <f t="shared" si="10"/>
+        <v>1.8355721998543286</v>
+      </c>
+      <c r="AS46">
+        <v>0.41522609930416121</v>
+      </c>
+    </row>
+    <row r="47" spans="31:45" x14ac:dyDescent="0.3">
+      <c r="AE47" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF47">
+        <v>1.1776877037793818</v>
+      </c>
+      <c r="AG47">
+        <v>0.57049016331182745</v>
+      </c>
+      <c r="AH47">
+        <v>0.31912886837985288</v>
+      </c>
+      <c r="AI47">
+        <v>0</v>
+      </c>
+      <c r="AJ47">
+        <v>0.64412061344635063</v>
+      </c>
+      <c r="AK47">
+        <v>6.1295580940860975E-2</v>
+      </c>
+      <c r="AL47">
+        <v>0.12329411811577708</v>
+      </c>
+      <c r="AM47">
+        <v>4.9266244801216393E-2</v>
+      </c>
+      <c r="AN47">
+        <v>1.8874925730159362</v>
+      </c>
+      <c r="AP47">
+        <f t="shared" si="10"/>
+        <v>2.1983575382069231</v>
+      </c>
+      <c r="AS47">
+        <v>0.2996504780125866</v>
+      </c>
+    </row>
+    <row r="48" spans="31:45" x14ac:dyDescent="0.3">
+      <c r="AE48" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF48">
+        <v>1.1099215617322973</v>
+      </c>
+      <c r="AG48">
+        <v>0</v>
+      </c>
+      <c r="AH48">
+        <v>1.3400249247540494</v>
+      </c>
+      <c r="AI48">
+        <v>1.054146888472042</v>
+      </c>
+      <c r="AJ48">
+        <v>0</v>
+      </c>
+      <c r="AK48">
+        <v>1.4122501848774365</v>
+      </c>
+      <c r="AL48">
+        <v>1.510352946918269</v>
+      </c>
+      <c r="AM48">
+        <v>0.6796730915433119</v>
+      </c>
+      <c r="AN48">
+        <v>4.0007168486438562</v>
+      </c>
+      <c r="AP48">
+        <f t="shared" si="10"/>
+        <v>3.3327295790299671</v>
+      </c>
+      <c r="AS48">
+        <v>-6.1736103896332217E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="31:45" x14ac:dyDescent="0.3">
+      <c r="AE49" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF49">
+        <v>0.37687073210213229</v>
+      </c>
+      <c r="AG49">
+        <v>2.7556583181346572E-2</v>
+      </c>
+      <c r="AH49">
+        <v>1.0189653548027497</v>
+      </c>
+      <c r="AI49">
+        <v>0.41258155819680903</v>
+      </c>
+      <c r="AJ49">
+        <v>0.48899283725024384</v>
+      </c>
+      <c r="AK49">
+        <v>4.3250161911871504E-2</v>
+      </c>
+      <c r="AL49">
+        <v>0.30909150444302452</v>
+      </c>
+      <c r="AM49">
+        <v>0.16991827288582798</v>
+      </c>
+      <c r="AN49">
+        <v>1.8874925730159362</v>
+      </c>
+      <c r="AP49">
+        <f t="shared" si="10"/>
+        <v>2.1759410786576785</v>
+      </c>
+      <c r="AS49">
+        <v>0.30679188083588205</v>
+      </c>
+    </row>
+    <row r="50" spans="31:45" x14ac:dyDescent="0.3">
+      <c r="AE50" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF50">
+        <v>0</v>
+      </c>
+      <c r="AG50">
+        <v>1.5088882686778121E-3</v>
+      </c>
+      <c r="AH50">
+        <v>1.2975277209671576</v>
+      </c>
+      <c r="AI50">
+        <v>0.92830850594282022</v>
+      </c>
+      <c r="AJ50">
+        <v>4.795091315926979E-2</v>
+      </c>
+      <c r="AK50">
+        <v>0.98072929505377571</v>
+      </c>
+      <c r="AL50">
+        <v>0.72007189816228145</v>
+      </c>
+      <c r="AM50">
+        <v>1.0295639729886858</v>
+      </c>
+      <c r="AN50">
+        <v>3.7619229136926617</v>
+      </c>
+      <c r="AP50">
+        <f t="shared" si="10"/>
+        <v>2.9610106565555161</v>
+      </c>
+      <c r="AS50">
+        <v>5.6685565529195903E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>